<commit_message>
Moved from webpack to plain tsc
- Moved all resources/ files to app/ folder
- Now translates Save dialog
</commit_message>
<xml_diff>
--- a/src/data/TDE5_en-US.xlsx
+++ b/src/data/TDE5_en-US.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas Obermann\Save\TDE app files\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas Obermann\Save\TDE app files\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="2468" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="2468" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="16" r:id="rId1"/>
@@ -2388,9 +2388,6 @@
     <t>White Mage</t>
   </si>
   <si>
-    <t>Gareth Academy of Sword and Staf</t>
-  </si>
-  <si>
     <t>{"id":"DISADV_34","tier":2,"sid":"protect the Middenrealm and the nobility, faith in the Twelvegods, truthfulness"}</t>
   </si>
   <si>
@@ -3616,6 +3613,9 @@
   </si>
   <si>
     <t>1?CT_1&amp;2?CT_2&amp;3?CT_14</t>
+  </si>
+  <si>
+    <t>Gareth Academy of Sword and Staff</t>
   </si>
 </sst>
 </file>
@@ -3737,7 +3737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="36">
     <dxf>
@@ -4270,7 +4270,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4572,7 +4572,7 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.73046875" bestFit="1" customWidth="1"/>
@@ -4674,7 +4674,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.46484375" style="2" customWidth="1"/>
@@ -5736,7 +5736,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1"/>
@@ -5875,7 +5875,7 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.1328125" customWidth="1"/>
     <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
@@ -6666,7 +6666,7 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
@@ -6804,7 +6804,7 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.9296875" bestFit="1" customWidth="1"/>
@@ -7151,7 +7151,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.19921875" bestFit="1" customWidth="1"/>
@@ -7270,11 +7270,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.1328125" customWidth="1"/>
     <col min="2" max="2" width="42.86328125" bestFit="1" customWidth="1"/>
@@ -7973,7 +7973,7 @@
         <v>247</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
@@ -8507,7 +8507,7 @@
       <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.86328125" bestFit="1" customWidth="1"/>
@@ -8694,7 +8694,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -9031,7 +9031,7 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.86328125" bestFit="1" customWidth="1"/>
@@ -9186,7 +9186,7 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
@@ -9269,7 +9269,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.19921875" bestFit="1" customWidth="1"/>
@@ -9288,7 +9288,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -9296,7 +9296,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -9304,7 +9304,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -9312,7 +9312,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -9320,7 +9320,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -9328,7 +9328,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -9344,7 +9344,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -9360,7 +9360,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -9368,7 +9368,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -9376,7 +9376,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -9384,7 +9384,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -9392,7 +9392,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -9400,7 +9400,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -9408,7 +9408,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -9424,7 +9424,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
@@ -9432,7 +9432,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -9440,7 +9440,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
@@ -9448,7 +9448,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
@@ -9456,7 +9456,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
@@ -9464,7 +9464,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
@@ -9472,7 +9472,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
@@ -9480,7 +9480,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
@@ -9488,7 +9488,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
@@ -9496,7 +9496,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
@@ -9504,7 +9504,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
@@ -9512,7 +9512,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
@@ -9520,7 +9520,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
@@ -9528,7 +9528,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -9536,7 +9536,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
@@ -9552,7 +9552,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
@@ -9560,7 +9560,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
@@ -9568,7 +9568,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -9576,7 +9576,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
@@ -9584,7 +9584,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
@@ -9592,7 +9592,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
@@ -9608,7 +9608,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
@@ -9616,7 +9616,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
@@ -9624,7 +9624,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
@@ -9632,7 +9632,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
@@ -9640,7 +9640,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
@@ -9648,7 +9648,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
@@ -9656,7 +9656,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
@@ -9664,7 +9664,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
@@ -9672,7 +9672,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
@@ -9680,7 +9680,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
@@ -9688,7 +9688,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
@@ -9696,7 +9696,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
@@ -9704,7 +9704,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
@@ -9712,7 +9712,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
@@ -9720,7 +9720,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
@@ -9728,7 +9728,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
@@ -9744,7 +9744,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
@@ -9752,7 +9752,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
@@ -9760,7 +9760,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
@@ -9768,7 +9768,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
@@ -9784,7 +9784,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
@@ -9792,7 +9792,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
@@ -9800,7 +9800,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
@@ -9808,7 +9808,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
@@ -9816,7 +9816,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
@@ -9824,7 +9824,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
@@ -9832,7 +9832,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
@@ -9840,7 +9840,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
@@ -9848,7 +9848,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
@@ -9856,7 +9856,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
@@ -9864,7 +9864,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
@@ -9872,7 +9872,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
@@ -9880,7 +9880,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
@@ -9888,7 +9888,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
@@ -9896,7 +9896,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
@@ -9904,7 +9904,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.45">
@@ -9912,7 +9912,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.45">
@@ -9920,7 +9920,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.45">
@@ -9928,7 +9928,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.45">
@@ -9936,7 +9936,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.45">
@@ -9952,7 +9952,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
@@ -9960,7 +9960,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.45">
@@ -9968,7 +9968,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.45">
@@ -9976,7 +9976,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.45">
@@ -9984,7 +9984,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.45">
@@ -9992,7 +9992,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.45">
@@ -10000,7 +10000,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
@@ -10008,7 +10008,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
@@ -10016,7 +10016,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
@@ -10024,7 +10024,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="23" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.45">
@@ -10032,7 +10032,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="23" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.45">
@@ -10040,7 +10040,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="23" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.45">
@@ -10048,7 +10048,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.45">
@@ -10056,7 +10056,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="23" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.45">
@@ -10064,7 +10064,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="23" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.45">
@@ -10072,7 +10072,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="24" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.45">
@@ -10080,7 +10080,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="24" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.45">
@@ -10088,7 +10088,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="24" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.45">
@@ -10096,7 +10096,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.45">
@@ -10104,7 +10104,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="24" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.45">
@@ -10112,7 +10112,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.45">
@@ -10120,7 +10120,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
@@ -10128,7 +10128,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
@@ -10136,7 +10136,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">
@@ -10144,7 +10144,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.45">
@@ -10152,7 +10152,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
@@ -10160,7 +10160,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
@@ -10168,7 +10168,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="23" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -10176,7 +10176,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
@@ -10184,7 +10184,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="23" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
@@ -10192,7 +10192,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="23" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
@@ -10200,7 +10200,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="23" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
@@ -10208,7 +10208,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="23" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
@@ -10216,7 +10216,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="23" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
@@ -10224,7 +10224,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="23" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
@@ -10232,7 +10232,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="23" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
@@ -10240,7 +10240,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="23" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
@@ -10248,7 +10248,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="23" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
@@ -10256,7 +10256,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="23" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
@@ -10264,7 +10264,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="23" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
@@ -10272,7 +10272,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="23" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
@@ -10280,7 +10280,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="23" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
@@ -10288,7 +10288,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="23" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
@@ -10296,7 +10296,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="23" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
@@ -10304,7 +10304,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="23" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
@@ -10312,7 +10312,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="23" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
@@ -10320,7 +10320,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="23" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
@@ -10328,7 +10328,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="23" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
@@ -10344,7 +10344,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="23" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
@@ -10352,7 +10352,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="23" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
@@ -10360,7 +10360,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="23" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
@@ -10368,7 +10368,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="23" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
@@ -10376,7 +10376,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="23" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
@@ -10384,7 +10384,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="23" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
@@ -10392,7 +10392,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="23" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
@@ -10400,7 +10400,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="23" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
@@ -10408,7 +10408,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="23" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
@@ -10416,7 +10416,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="23" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
@@ -10424,7 +10424,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.45">
@@ -10432,7 +10432,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.45">
@@ -10440,7 +10440,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.45">
@@ -10448,7 +10448,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.45">
@@ -10456,7 +10456,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.45">
@@ -10464,7 +10464,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.45">
@@ -10472,7 +10472,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.45">
@@ -10480,7 +10480,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.45">
@@ -10488,7 +10488,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.45">
@@ -10496,7 +10496,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.45">
@@ -10512,7 +10512,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="23" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.45">
@@ -10520,7 +10520,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.45">
@@ -10528,7 +10528,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.45">
@@ -10536,7 +10536,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.45">
@@ -10544,7 +10544,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="23" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.45">
@@ -10552,7 +10552,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.45">
@@ -10560,7 +10560,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="23" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.45">
@@ -10568,7 +10568,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="23" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.45">
@@ -10576,7 +10576,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="23" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.45">
@@ -10584,7 +10584,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="23" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.45">
@@ -10592,7 +10592,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="23" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.45">
@@ -10600,7 +10600,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="23" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.45">
@@ -10608,7 +10608,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="23" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.45">
@@ -10616,7 +10616,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="23" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.45">
@@ -10624,7 +10624,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="23" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.45">
@@ -10632,7 +10632,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="24" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.45">
@@ -10640,7 +10640,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="23" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.45">
@@ -10648,7 +10648,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="23" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.45">
@@ -10656,7 +10656,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="23" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.45">
@@ -10664,7 +10664,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="23" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.45">
@@ -10672,7 +10672,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="23" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.45">
@@ -10680,7 +10680,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="23" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.45">
@@ -10688,7 +10688,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="23" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.45">
@@ -10696,7 +10696,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="23" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.45">
@@ -10704,7 +10704,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="23" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.45">
@@ -10712,7 +10712,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="23" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.45">
@@ -10720,7 +10720,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="23" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.45">
@@ -10728,7 +10728,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="23" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.45">
@@ -10736,7 +10736,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="23" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.45">
@@ -10744,7 +10744,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="23" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.45">
@@ -10752,7 +10752,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="23" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
@@ -10760,7 +10760,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="23" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.45">
@@ -10768,7 +10768,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="23" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.45">
@@ -10776,7 +10776,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="23" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.45">
@@ -10784,7 +10784,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="23" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.45">
@@ -10792,7 +10792,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="23" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
@@ -10800,7 +10800,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="23" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.45">
@@ -10808,7 +10808,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="23" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
@@ -10816,7 +10816,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="23" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.45">
@@ -10824,7 +10824,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="23" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.45">
@@ -10832,7 +10832,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="23" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.45">
@@ -10840,7 +10840,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="23" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.45">
@@ -10848,7 +10848,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="23" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.45">
@@ -10856,7 +10856,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="23" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.45">
@@ -10864,7 +10864,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="23" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.45">
@@ -10872,7 +10872,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="23" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.45">
@@ -10880,7 +10880,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="23" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.45">
@@ -10888,7 +10888,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="23" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.45">
@@ -10896,7 +10896,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="23" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.45">
@@ -10904,7 +10904,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="23" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.45">
@@ -10912,7 +10912,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="23" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.45">
@@ -10920,7 +10920,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="23" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.45">
@@ -10928,7 +10928,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="23" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.45">
@@ -10936,7 +10936,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="23" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.45">
@@ -10952,7 +10952,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="23" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.45">
@@ -10960,7 +10960,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="23" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.45">
@@ -10968,7 +10968,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="23" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.45">
@@ -10976,7 +10976,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="23" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.45">
@@ -10984,7 +10984,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="23" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.45">
@@ -10992,7 +10992,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="23" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.45">
@@ -11008,7 +11008,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="23" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.45">
@@ -11016,7 +11016,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="24" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.45">
@@ -11024,7 +11024,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="24" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.45">
@@ -11032,7 +11032,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="24" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.45">
@@ -11040,7 +11040,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="24" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.45">
@@ -11048,7 +11048,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.45">
@@ -11056,7 +11056,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="24" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.45">
@@ -11064,7 +11064,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="24" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.45">
@@ -11072,7 +11072,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="24" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.45">
@@ -11080,7 +11080,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="23" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.45">
@@ -11088,7 +11088,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="23" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.45">
@@ -11096,7 +11096,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="23" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.45">
@@ -11104,7 +11104,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="23" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.45">
@@ -11112,7 +11112,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="23" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.45">
@@ -11120,7 +11120,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="23" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.45">
@@ -11128,7 +11128,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="23" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.45">
@@ -11136,7 +11136,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="23" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.45">
@@ -11144,7 +11144,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="23" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.45">
@@ -11152,7 +11152,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="23" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.45">
@@ -11160,7 +11160,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="23" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.45">
@@ -11168,7 +11168,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="23" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.45">
@@ -11176,7 +11176,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="23" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.45">
@@ -11184,7 +11184,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="23" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.45">
@@ -11200,7 +11200,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="23" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.45">
@@ -11208,7 +11208,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="23" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.45">
@@ -11216,7 +11216,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="23" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.45">
@@ -11224,7 +11224,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="23" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.45">
@@ -11232,7 +11232,7 @@
         <v>244</v>
       </c>
       <c r="B245" s="23" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.45">
@@ -11240,7 +11240,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="23" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.45">
@@ -11248,7 +11248,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.45">
@@ -11256,7 +11256,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="23" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.45">
@@ -11264,7 +11264,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="23" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.45">
@@ -11272,7 +11272,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="23" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.45">
@@ -11280,7 +11280,7 @@
         <v>250</v>
       </c>
       <c r="B251" s="23" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.45">
@@ -11288,7 +11288,7 @@
         <v>251</v>
       </c>
       <c r="B252" s="23" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.45">
@@ -11296,7 +11296,7 @@
         <v>252</v>
       </c>
       <c r="B253" s="23" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.45">
@@ -11304,7 +11304,7 @@
         <v>253</v>
       </c>
       <c r="B254" s="23" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.45">
@@ -11312,7 +11312,7 @@
         <v>254</v>
       </c>
       <c r="B255" s="23" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.45">
@@ -11320,7 +11320,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="23" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.45">
@@ -11328,7 +11328,7 @@
         <v>256</v>
       </c>
       <c r="B257" s="23" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.45">
@@ -11344,7 +11344,7 @@
         <v>258</v>
       </c>
       <c r="B259" s="23" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.45">
@@ -11360,7 +11360,7 @@
         <v>260</v>
       </c>
       <c r="B261" s="23" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.45">
@@ -11368,7 +11368,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="23" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.45">
@@ -11376,7 +11376,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="23" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.45">
@@ -11392,7 +11392,7 @@
         <v>264</v>
       </c>
       <c r="B265" s="23" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.45">
@@ -11400,7 +11400,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="23" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.45">
@@ -11408,7 +11408,7 @@
         <v>266</v>
       </c>
       <c r="B267" s="23" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.45">
@@ -11416,7 +11416,7 @@
         <v>267</v>
       </c>
       <c r="B268" s="23" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.45">
@@ -11424,7 +11424,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="23" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.45">
@@ -11432,7 +11432,7 @@
         <v>269</v>
       </c>
       <c r="B270" s="23" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.45">
@@ -11440,7 +11440,7 @@
         <v>270</v>
       </c>
       <c r="B271" s="23" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.45">
@@ -11448,7 +11448,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="23" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.45">
@@ -11456,7 +11456,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="23" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.45">
@@ -11464,7 +11464,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="23" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.45">
@@ -11488,7 +11488,7 @@
         <v>276</v>
       </c>
       <c r="B277" s="23" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.45">
@@ -11496,7 +11496,7 @@
         <v>277</v>
       </c>
       <c r="B278" s="23" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.45">
@@ -11504,7 +11504,7 @@
         <v>278</v>
       </c>
       <c r="B279" s="23" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.45">
@@ -11512,7 +11512,7 @@
         <v>279</v>
       </c>
       <c r="B280" s="23" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.45">
@@ -11520,7 +11520,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="23" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.45">
@@ -11528,7 +11528,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="23" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.45">
@@ -11536,7 +11536,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="23" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.45">
@@ -11544,7 +11544,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="23" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.45">
@@ -11552,7 +11552,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="23" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.45">
@@ -11560,7 +11560,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="23" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.45">
@@ -11568,7 +11568,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="23" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.45">
@@ -11576,7 +11576,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="23" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.45">
@@ -11584,7 +11584,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="23" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.45">
@@ -11592,7 +11592,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="23" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.45">
@@ -11600,7 +11600,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="23" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.45">
@@ -11608,7 +11608,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="23" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.45">
@@ -11616,7 +11616,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="23" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.45">
@@ -11640,7 +11640,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="23" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.45">
@@ -11648,7 +11648,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="23" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.45">
@@ -11656,7 +11656,7 @@
         <v>297</v>
       </c>
       <c r="B298" s="23" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.45">
@@ -11672,7 +11672,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="23" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.45">
@@ -11680,7 +11680,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="23" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.45">
@@ -11688,7 +11688,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="23" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.45">
@@ -11720,7 +11720,7 @@
         <v>305</v>
       </c>
       <c r="B306" s="23" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.45">
@@ -11760,7 +11760,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="23" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.45">
@@ -11768,7 +11768,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="23" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.45">
@@ -11784,7 +11784,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="23" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.45">
@@ -11800,7 +11800,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="23" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.45">
@@ -11808,7 +11808,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="23" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.45">
@@ -11824,7 +11824,7 @@
         <v>318</v>
       </c>
       <c r="B319" s="23" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.45">
@@ -11832,7 +11832,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="23" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.45">
@@ -11840,7 +11840,7 @@
         <v>320</v>
       </c>
       <c r="B321" s="23" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.45">
@@ -11848,7 +11848,7 @@
         <v>321</v>
       </c>
       <c r="B322" s="23" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.45">
@@ -11856,7 +11856,7 @@
         <v>322</v>
       </c>
       <c r="B323" s="23" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.45">
@@ -11864,7 +11864,7 @@
         <v>323</v>
       </c>
       <c r="B324" s="23" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.45">
@@ -11872,7 +11872,7 @@
         <v>324</v>
       </c>
       <c r="B325" s="23" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.45">
@@ -11880,7 +11880,7 @@
         <v>325</v>
       </c>
       <c r="B326" s="23" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.45">
@@ -11904,7 +11904,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="23" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.45">
@@ -11912,7 +11912,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="23" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.45">
@@ -11920,7 +11920,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="23" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.45">
@@ -11928,7 +11928,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="23" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.45">
@@ -11936,7 +11936,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="23" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.45">
@@ -11944,7 +11944,7 @@
         <v>333</v>
       </c>
       <c r="B334" s="23" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.45">
@@ -11952,7 +11952,7 @@
         <v>334</v>
       </c>
       <c r="B335" s="23" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.45">
@@ -11960,7 +11960,7 @@
         <v>335</v>
       </c>
       <c r="B336" s="23" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.45">
@@ -11968,7 +11968,7 @@
         <v>336</v>
       </c>
       <c r="B337" s="23" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.45">
@@ -11976,7 +11976,7 @@
         <v>337</v>
       </c>
       <c r="B338" s="23" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.45">
@@ -11984,7 +11984,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="23" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.45">
@@ -11992,7 +11992,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="23" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.45">
@@ -12000,7 +12000,7 @@
         <v>340</v>
       </c>
       <c r="B341" s="23" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.45">
@@ -12008,7 +12008,7 @@
         <v>341</v>
       </c>
       <c r="B342" s="23" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.45">
@@ -12016,7 +12016,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="23" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.45">
@@ -12024,7 +12024,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="23" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.45">
@@ -12032,7 +12032,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="23" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.45">
@@ -12040,7 +12040,7 @@
         <v>345</v>
       </c>
       <c r="B346" s="23" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.45">
@@ -12048,7 +12048,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="23" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.45">
@@ -12056,7 +12056,7 @@
         <v>347</v>
       </c>
       <c r="B348" s="23" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.45">
@@ -12064,7 +12064,7 @@
         <v>348</v>
       </c>
       <c r="B349" s="23" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.45">
@@ -12072,7 +12072,7 @@
         <v>349</v>
       </c>
       <c r="B350" s="23" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.45">
@@ -12080,7 +12080,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="23" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.45">
@@ -12088,7 +12088,7 @@
         <v>351</v>
       </c>
       <c r="B352" s="23" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.45">
@@ -12096,7 +12096,7 @@
         <v>352</v>
       </c>
       <c r="B353" s="23" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.45">
@@ -12104,7 +12104,7 @@
         <v>353</v>
       </c>
       <c r="B354" s="23" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.45">
@@ -12112,7 +12112,7 @@
         <v>354</v>
       </c>
       <c r="B355" s="23" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.45">
@@ -12120,7 +12120,7 @@
         <v>355</v>
       </c>
       <c r="B356" s="23" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.45">
@@ -12128,7 +12128,7 @@
         <v>356</v>
       </c>
       <c r="B357" s="23" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.45">
@@ -12136,7 +12136,7 @@
         <v>357</v>
       </c>
       <c r="B358" s="23" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.45">
@@ -12144,7 +12144,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="23" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.45">
@@ -12152,7 +12152,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="23" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.45">
@@ -12160,7 +12160,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="23" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.45">
@@ -12168,7 +12168,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="23" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.45">
@@ -12176,7 +12176,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="23" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.45">
@@ -12184,7 +12184,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="23" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.45">
@@ -12200,7 +12200,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="23" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.45">
@@ -12208,7 +12208,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="23" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.45">
@@ -12216,7 +12216,7 @@
         <v>367</v>
       </c>
       <c r="B368" s="23" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.45">
@@ -12224,7 +12224,7 @@
         <v>368</v>
       </c>
       <c r="B369" s="23" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.45">
@@ -12232,7 +12232,7 @@
         <v>369</v>
       </c>
       <c r="B370" s="23" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.45">
@@ -12240,7 +12240,7 @@
         <v>370</v>
       </c>
       <c r="B371" s="23" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.45">
@@ -12248,7 +12248,7 @@
         <v>371</v>
       </c>
       <c r="B372" s="23" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.45">
@@ -12256,7 +12256,7 @@
         <v>372</v>
       </c>
       <c r="B373" s="23" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.45">
@@ -12264,7 +12264,7 @@
         <v>373</v>
       </c>
       <c r="B374" s="23" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.45">
@@ -12272,7 +12272,7 @@
         <v>374</v>
       </c>
       <c r="B375" s="23" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.45">
@@ -12280,7 +12280,7 @@
         <v>375</v>
       </c>
       <c r="B376" s="23" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.45">
@@ -12288,7 +12288,7 @@
         <v>376</v>
       </c>
       <c r="B377" s="23" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.45">
@@ -12296,7 +12296,7 @@
         <v>377</v>
       </c>
       <c r="B378" s="24" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.45">
@@ -12304,7 +12304,7 @@
         <v>378</v>
       </c>
       <c r="B379" s="24" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.45">
@@ -12312,7 +12312,7 @@
         <v>379</v>
       </c>
       <c r="B380" s="24" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.45">
@@ -12320,7 +12320,7 @@
         <v>380</v>
       </c>
       <c r="B381" s="24" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.45">
@@ -12328,7 +12328,7 @@
         <v>381</v>
       </c>
       <c r="B382" s="24" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
   </sheetData>
@@ -12344,7 +12344,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.73046875" bestFit="1" customWidth="1"/>
@@ -12467,7 +12467,7 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.19921875" bestFit="1" customWidth="1"/>
@@ -12690,11 +12690,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.73046875" bestFit="1" customWidth="1"/>
@@ -13037,10 +13037,10 @@
         <v>780</v>
       </c>
       <c r="C25" s="21" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>781</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>782</v>
       </c>
       <c r="E25" s="16">
         <v>153</v>
@@ -13051,11 +13051,11 @@
         <v>26</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E26" s="16">
         <v>154</v>
@@ -13066,11 +13066,11 @@
         <v>27</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E27" s="16">
         <v>155</v>
@@ -13081,11 +13081,11 @@
         <v>28</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E28" s="16">
         <v>156</v>
@@ -13096,11 +13096,11 @@
         <v>29</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E29" s="16">
         <v>157</v>
@@ -13111,11 +13111,11 @@
         <v>30</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E30" s="16">
         <v>158</v>
@@ -13126,11 +13126,11 @@
         <v>31</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E31" s="16">
         <v>159</v>
@@ -13150,7 +13150,7 @@
       <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.53125" bestFit="1" customWidth="1"/>
@@ -13169,7 +13169,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -13185,7 +13185,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -13193,7 +13193,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -13201,7 +13201,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -13209,7 +13209,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -13217,7 +13217,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
@@ -13225,7 +13225,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -13233,7 +13233,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -13241,7 +13241,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -13249,7 +13249,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -13257,7 +13257,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -13265,7 +13265,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -13273,7 +13273,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -13281,7 +13281,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -13289,7 +13289,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -13297,7 +13297,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
@@ -13305,7 +13305,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
@@ -13313,7 +13313,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -13329,7 +13329,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
@@ -13337,7 +13337,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
@@ -13345,7 +13345,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
@@ -13361,7 +13361,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
@@ -13369,7 +13369,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
@@ -13377,7 +13377,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
@@ -13385,7 +13385,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
@@ -13393,7 +13393,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
@@ -13401,7 +13401,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
@@ -13409,7 +13409,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -13417,7 +13417,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
@@ -13425,7 +13425,7 @@
         <v>38</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
@@ -13441,7 +13441,7 @@
         <v>40</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
@@ -13449,7 +13449,7 @@
         <v>41</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -13457,7 +13457,7 @@
         <v>42</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
@@ -13465,7 +13465,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
@@ -13473,7 +13473,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
@@ -13481,7 +13481,7 @@
         <v>45</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
@@ -13489,7 +13489,7 @@
         <v>46</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
@@ -13497,7 +13497,7 @@
         <v>47</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
@@ -13505,7 +13505,7 @@
         <v>48</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
@@ -13513,7 +13513,7 @@
         <v>49</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
@@ -13521,7 +13521,7 @@
         <v>50</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
@@ -13529,7 +13529,7 @@
         <v>51</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
@@ -13537,7 +13537,7 @@
         <v>52</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
@@ -13545,7 +13545,7 @@
         <v>54</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
@@ -13553,7 +13553,7 @@
         <v>55</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
@@ -13585,7 +13585,7 @@
         <v>59</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
@@ -13593,7 +13593,7 @@
         <v>60</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
@@ -13609,7 +13609,7 @@
         <v>62</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
@@ -13617,7 +13617,7 @@
         <v>63</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
@@ -13625,7 +13625,7 @@
         <v>64</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
@@ -13633,7 +13633,7 @@
         <v>65</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
@@ -13641,7 +13641,7 @@
         <v>66</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
@@ -13649,7 +13649,7 @@
         <v>67</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
   </sheetData>
@@ -13665,7 +13665,7 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.1328125" style="11" customWidth="1"/>
     <col min="2" max="2" width="35.796875" style="11" bestFit="1" customWidth="1"/>
@@ -13976,7 +13976,7 @@
         <v>523</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D30" s="9"/>
     </row>
@@ -14240,7 +14240,7 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.1328125" customWidth="1"/>
     <col min="2" max="2" width="35.796875" bestFit="1" customWidth="1"/>
@@ -14634,7 +14634,7 @@
         <v>590</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>591</v>
@@ -14882,7 +14882,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Added language specializations and fixed tier-based dependencies
</commit_message>
<xml_diff>
--- a/src/data/TDE5_en-US.xlsx
+++ b/src/data/TDE5_en-US.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="2468" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="2468" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="16" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3756" uniqueCount="2441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3759" uniqueCount="2444">
   <si>
     <t>id</t>
   </si>
@@ -9778,6 +9778,15 @@
   </si>
   <si>
     <t>To buy an elf bow during hero creation, the character must be from an elven culture.</t>
+  </si>
+  <si>
+    <t>Language Specialization</t>
+  </si>
+  <si>
+    <t>Knowing and using a Language Specialization grants the hero a bonus of 1 for *Fast-Talk (Hard Sell)*, as long as the other person speaks the same dialect. The GM decides if the bonus applies. A character with a dialect might suffer a penalty of 1 in some situations, such as when the other person has trouble understanding what is being said.\nThe use of this optional rule makes the game a little more complex.</t>
+  </si>
+  <si>
+    <t>the relevant language at Level III</t>
   </si>
 </sst>
 </file>
@@ -9892,12 +9901,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10003,13 +10013,252 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Erklärender Text 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{B06DF788-D2AB-4699-8EA8-C2CC1DBAADEC}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{3F62BF4F-0F52-4DDA-A66D-D96FCAAA1927}"/>
   </cellStyles>
   <dxfs count="140">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -10245,25 +10494,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -10273,31 +10503,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -10317,113 +10522,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -10470,9 +10568,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -10482,74 +10577,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -11205,72 +11232,72 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{20810958-2B1F-489B-85BB-A71CA319D3BE}" name="Tabelle12" displayName="Tabelle12" ref="A1:H13" totalsRowShown="0" headerRowDxfId="24" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{20810958-2B1F-489B-85BB-A71CA319D3BE}" name="Tabelle12" displayName="Tabelle12" ref="A1:H13" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A1:H13" xr:uid="{FA47A379-2233-4074-9AB1-152EE983B10E}"/>
   <sortState ref="A2:H13">
     <sortCondition ref="A1:A13"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{80423AAF-9A13-4048-90DA-956235CA7B70}" name="id" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{53F47762-1B13-471B-AED9-BF2C490D5CD8}" name="name" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{D0C580B0-3F04-439D-9F30-4147BC1B68C0}" name="effect" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{75585642-4807-407A-9124-0B604AF9D272}" name="range" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{5CF4ADF6-B805-4539-B1EB-BEA810029856}" name="duration" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{8883C844-90D8-4ED4-97EB-136CF8FED8B1}" name="target" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{E51FF880-E2D0-4954-8C6C-29177C28EDBC}" name="note" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{1C430D7A-5610-4443-BFFF-4336DE092717}" name="src" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{80423AAF-9A13-4048-90DA-956235CA7B70}" name="id" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{53F47762-1B13-471B-AED9-BF2C490D5CD8}" name="name" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{D0C580B0-3F04-439D-9F30-4147BC1B68C0}" name="effect" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{75585642-4807-407A-9124-0B604AF9D272}" name="range" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{5CF4ADF6-B805-4539-B1EB-BEA810029856}" name="duration" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{8883C844-90D8-4ED4-97EB-136CF8FED8B1}" name="target" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{E51FF880-E2D0-4954-8C6C-29177C28EDBC}" name="note" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{1C430D7A-5610-4443-BFFF-4336DE092717}" name="src" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{A4AF9304-CECC-4706-BE3D-6C02E19EB7DE}" name="Tabelle14" displayName="Tabelle14" ref="A1:M41" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{A4AF9304-CECC-4706-BE3D-6C02E19EB7DE}" name="Tabelle14" displayName="Tabelle14" ref="A1:M41" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:M41" xr:uid="{7C560F19-2483-4764-A4E9-59A9B4A4DAC4}"/>
   <sortState ref="A2:M41">
     <sortCondition ref="A1:A41"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{38B0EF5B-69CE-4E41-B5E8-D46D558C4B98}" name="id" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{D6AA4D77-9FBB-4EA0-BBAD-AD239EB9AAD5}" name="name" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{D2756D7F-8900-4980-B57E-7CE762BEFFDE}" name="effect" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{99685749-C1CC-4C60-AAD7-1C87F2BA9A75}" name="castingtime" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{7EEE05E4-4512-407B-842A-1FD00585DDD2}" name="castingtimeShort" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{9DFECF77-BCF0-4763-9062-58BFD91CF7F9}" name="kpcost" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{3D4EF3CF-F964-45A4-B7C4-DBDEFC1C81A6}" name="kpcostShort" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{CCE83C8E-D682-41C8-8786-C98691C246AD}" name="range" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{7652F0CC-E291-423C-AC62-F06CE8503F50}" name="rangeShort" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{2BE682CA-1853-4237-8DD1-CEC3E68129BD}" name="duration" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{CA193524-7BA2-41F8-AFCF-1E68017E2279}" name="durationShort" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{474BE732-F74C-44A8-BC43-96E09F985B63}" name="target" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{22BBA61D-F2BE-4593-AA32-78E151203060}" name="src" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{38B0EF5B-69CE-4E41-B5E8-D46D558C4B98}" name="id" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{D6AA4D77-9FBB-4EA0-BBAD-AD239EB9AAD5}" name="name" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{D2756D7F-8900-4980-B57E-7CE762BEFFDE}" name="effect" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{99685749-C1CC-4C60-AAD7-1C87F2BA9A75}" name="castingtime" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{7EEE05E4-4512-407B-842A-1FD00585DDD2}" name="castingtimeShort" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{9DFECF77-BCF0-4763-9062-58BFD91CF7F9}" name="kpcost" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{3D4EF3CF-F964-45A4-B7C4-DBDEFC1C81A6}" name="kpcostShort" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{CCE83C8E-D682-41C8-8786-C98691C246AD}" name="range" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{7652F0CC-E291-423C-AC62-F06CE8503F50}" name="rangeShort" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{2BE682CA-1853-4237-8DD1-CEC3E68129BD}" name="duration" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{CA193524-7BA2-41F8-AFCF-1E68017E2279}" name="durationShort" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{474BE732-F74C-44A8-BC43-96E09F985B63}" name="target" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{22BBA61D-F2BE-4593-AA32-78E151203060}" name="src" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE1F12EC-7104-418A-9BFC-32F94E60D1E9}" name="Tabelle13" displayName="Tabelle13" ref="A1:G13" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE1F12EC-7104-418A-9BFC-32F94E60D1E9}" name="Tabelle13" displayName="Tabelle13" ref="A1:G13" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:G13" xr:uid="{5CD72CB2-8095-4D11-AA09-6E7628D67F6C}"/>
   <sortState ref="A2:G13">
     <sortCondition ref="B1:B13"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{75CB1DE0-E276-4C7F-BCC6-FF2FA18B017D}" name="id" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{6B251442-2574-4230-AB18-D00D65F0DF9A}" name="name" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{E1197E89-64F9-4FC2-A9B4-4BC1813A85B6}" name="effect" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{C0232011-1F33-4ACB-AA8C-5B870FAB1352}" name="range" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{A95BD016-CF17-4F91-A309-2DE22B395A7A}" name="duration" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{2C7B8E03-7DF4-4F22-90E4-7035A2F0168B}" name="target" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{6FA15D05-BB98-49DB-B47D-2F14FEAFDF45}" name="src" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{75CB1DE0-E276-4C7F-BCC6-FF2FA18B017D}" name="id" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{6B251442-2574-4230-AB18-D00D65F0DF9A}" name="name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{E1197E89-64F9-4FC2-A9B4-4BC1813A85B6}" name="effect" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{C0232011-1F33-4ACB-AA8C-5B870FAB1352}" name="range" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{A95BD016-CF17-4F91-A309-2DE22B395A7A}" name="duration" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{2C7B8E03-7DF4-4F22-90E4-7035A2F0168B}" name="target" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{6FA15D05-BB98-49DB-B47D-2F14FEAFDF45}" name="src" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table2" displayName="Table2" ref="A1:W121" totalsRowShown="0" headerRowDxfId="45">
-  <autoFilter ref="A1:W121" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table2" displayName="Table2" ref="A1:W122" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:W122" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -11296,9 +11323,9 @@
     <filterColumn colId="22" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="sel" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="sel" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="input"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="nameInWiki"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="rules"/>
@@ -11325,7 +11352,7 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{23FB0876-5312-4CF4-A3ED-A9E081662530}" name="Tabelle10" displayName="Tabelle10" ref="A1:G382" totalsRowShown="0" headerRowDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{23FB0876-5312-4CF4-A3ED-A9E081662530}" name="Tabelle10" displayName="Tabelle10" ref="A1:G382" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:G382" xr:uid="{8EA38458-CF38-4B8F-90A8-E0991E0382F0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11334,13 +11361,13 @@
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B9AA81B7-8A64-4E82-9669-9D0FF8515AFC}" name="id" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{756DB8FB-83BA-4370-9112-C04F1AC7B4F1}" name="name" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{3F5C0939-9CF7-421A-8CAC-010D3F3E38A7}" name="note" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{4BAAB64F-94E7-4F1C-AE98-BA763FE5AC60}" name="rules" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{8B1B9365-52B9-4D00-AE3A-B0A3DF58603A}" name="advantage" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{1A0E8832-34C7-4BD0-A4F1-E8AC8CDBEA7B}" name="disadvantage" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{056266E9-8DF6-44B7-9E87-B389BD9EAE34}" name="src" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{B9AA81B7-8A64-4E82-9669-9D0FF8515AFC}" name="id" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{756DB8FB-83BA-4370-9112-C04F1AC7B4F1}" name="name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{3F5C0939-9CF7-421A-8CAC-010D3F3E38A7}" name="note" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{4BAAB64F-94E7-4F1C-AE98-BA763FE5AC60}" name="rules" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8B1B9365-52B9-4D00-AE3A-B0A3DF58603A}" name="advantage" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{1A0E8832-34C7-4BD0-A4F1-E8AC8CDBEA7B}" name="disadvantage" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{056266E9-8DF6-44B7-9E87-B389BD9EAE34}" name="src" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20463,11 +20490,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:W121"/>
+  <dimension ref="A1:W122"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -24480,6 +24507,41 @@
       <c r="V121" s="25"/>
       <c r="W121" s="25">
         <v>318</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A122" s="43">
+        <v>699</v>
+      </c>
+      <c r="B122" s="46" t="s">
+        <v>2441</v>
+      </c>
+      <c r="C122" s="23"/>
+      <c r="D122" s="41"/>
+      <c r="E122" s="42"/>
+      <c r="F122" s="42" t="s">
+        <v>2442</v>
+      </c>
+      <c r="G122" s="42"/>
+      <c r="H122" s="42"/>
+      <c r="I122" s="44"/>
+      <c r="J122" s="45"/>
+      <c r="K122" s="42"/>
+      <c r="L122" s="42"/>
+      <c r="M122" s="42"/>
+      <c r="N122" s="42"/>
+      <c r="O122" s="42"/>
+      <c r="P122" s="42"/>
+      <c r="Q122" s="41"/>
+      <c r="R122" s="41"/>
+      <c r="S122" s="42" t="s">
+        <v>2443</v>
+      </c>
+      <c r="T122" s="42"/>
+      <c r="U122" s="42"/>
+      <c r="V122" s="42"/>
+      <c r="W122" s="43">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -25256,7 +25318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G382"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>